<commit_message>
Massive Organization of the Entire Repo for Sprint 4. Completed (#47 & #48)
*Changed the entire routing system, to use appropriate urls so that the page reloading does not reset the page the user is currently.
*Completed US-18: Profile Editing (#47)
*Completed US-19: Deleting Documents (#48)
*Added unit tests for multiple views (nav, button, comments-modal, sidebar)
*Reorganized the folder structure to be organized into directories according to the part of the website they belong to
*Added comments to many of the files (beautified the files)
*Made method naming consistent across all files
*Added animations to both the comment modal and upload modal
*Added api routes for updating user info and deleting documents
*Re-authenticated the user when their information changes
*Removed unused dependencies
*Created reset script to erase all db tables and documents uploaded to the server
Pull request: #58
</commit_message>
<xml_diff>
--- a/Documentation/BurndownChart.xlsx
+++ b/Documentation/BurndownChart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="440" windowWidth="51120" windowHeight="28360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="44420" yWindow="2940" windowWidth="32280" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Task Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="111">
   <si>
     <t>Create the login/signup page</t>
   </si>
@@ -254,6 +254,114 @@
   <si>
     <t>Style the comment area so it looks nice for the user</t>
   </si>
+  <si>
+    <t>US-19: Deleting Documents (6)</t>
+  </si>
+  <si>
+    <t>US-18: Profile Editing (7)</t>
+  </si>
+  <si>
+    <t>US-17: User Role (3)</t>
+  </si>
+  <si>
+    <t>US-15: Profile Statistics (4)</t>
+  </si>
+  <si>
+    <t>US-05: Censoring Comments (5)</t>
+  </si>
+  <si>
+    <t>US-04: Leaving Comments on Documents (8)</t>
+  </si>
+  <si>
+    <t>Create font-end button to delete document</t>
+  </si>
+  <si>
+    <t>Send a http request with document to delete</t>
+  </si>
+  <si>
+    <t>Delete document on the server</t>
+  </si>
+  <si>
+    <t>Create font-end button and editing view</t>
+  </si>
+  <si>
+    <t>Style the front end views</t>
+  </si>
+  <si>
+    <t>Send http request with new data to the server</t>
+  </si>
+  <si>
+    <t>Update the database with new information</t>
+  </si>
+  <si>
+    <t>Create font-end section for dropdown</t>
+  </si>
+  <si>
+    <t>Style front-end section</t>
+  </si>
+  <si>
+    <t>Add verification on the server</t>
+  </si>
+  <si>
+    <t>Add role attribute to user</t>
+  </si>
+  <si>
+    <t>Load the role on the profile</t>
+  </si>
+  <si>
+    <t>Determine statistics criteria</t>
+  </si>
+  <si>
+    <t>Create front-end list or table to hold statistics</t>
+  </si>
+  <si>
+    <t>Style the front-end</t>
+  </si>
+  <si>
+    <t>Create backend api routes for the needed data</t>
+  </si>
+  <si>
+    <t>Create http requests to load data onto the frontend</t>
+  </si>
+  <si>
+    <t>Decide which words should be sensored</t>
+  </si>
+  <si>
+    <t>Use a library or a regex pattern to sensor the users comment before it is save to the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send a HTTP request to load comments from the database that already on a document </t>
+  </si>
+  <si>
+    <t>Send a HTTP request to send comments to save in the database</t>
+  </si>
+  <si>
+    <t>Associate comments to a document and user</t>
+  </si>
+  <si>
+    <t>Always make comments scroll to bottom</t>
+  </si>
+  <si>
+    <t>Update comments with new comment</t>
+  </si>
+  <si>
+    <t>SPRINT 4</t>
+  </si>
+  <si>
+    <t>US-16: Profile Biography (2)</t>
+  </si>
+  <si>
+    <t>Create font-end section for the biography</t>
+  </si>
+  <si>
+    <t>Style front-end section of the biography</t>
+  </si>
+  <si>
+    <t>Add biography attribute to user object in the database</t>
+  </si>
+  <si>
+    <t>Create http request to load biography from server</t>
+  </si>
 </sst>
 </file>
 
@@ -344,7 +452,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,8 +549,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD882BF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -842,6 +962,171 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -850,7 +1135,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -969,6 +1254,30 @@
     <xf numFmtId="164" fontId="3" fillId="14" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="16" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="16" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="10" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="17" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="18" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -979,6 +1288,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -993,8 +1311,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FFD882BF"/>
+      <color rgb="FF42929C"/>
       <color rgb="FFFF86FA"/>
-      <color rgb="FF42929C"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1167,8 +1486,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-745533664"/>
-        <c:axId val="-743356768"/>
+        <c:axId val="-1886781392"/>
+        <c:axId val="-1886785600"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1361,8 +1680,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-743078064"/>
-        <c:axId val="-743075744"/>
+        <c:axId val="-1885721792"/>
+        <c:axId val="-1885719472"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1456,11 +1775,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-745533664"/>
-        <c:axId val="-743356768"/>
+        <c:axId val="-1886781392"/>
+        <c:axId val="-1886785600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-743078064"/>
+        <c:axId val="-1885721792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1503,7 +1822,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-743075744"/>
+        <c:crossAx val="-1885719472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1511,7 +1830,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-743075744"/>
+        <c:axId val="-1885719472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1631,12 +1950,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-743078064"/>
+        <c:crossAx val="-1885721792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-743356768"/>
+        <c:axId val="-1886785600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25.0"/>
@@ -1737,12 +2056,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-745533664"/>
+        <c:crossAx val="-1886781392"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-745533664"/>
+        <c:axId val="-1886781392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1751,7 +2070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-743356768"/>
+        <c:crossAx val="-1886785600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2018,8 +2337,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-743949408"/>
-        <c:axId val="-744111040"/>
+        <c:axId val="-1885670496"/>
+        <c:axId val="-1885674256"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2250,8 +2569,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-743266528"/>
-        <c:axId val="-743264208"/>
+        <c:axId val="-1885680768"/>
+        <c:axId val="-1885678016"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2366,11 +2685,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-743949408"/>
-        <c:axId val="-744111040"/>
+        <c:axId val="-1885670496"/>
+        <c:axId val="-1885674256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-743266528"/>
+        <c:axId val="-1885680768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2413,7 +2732,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-743264208"/>
+        <c:crossAx val="-1885678016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2421,7 +2740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-743264208"/>
+        <c:axId val="-1885678016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2541,12 +2860,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-743266528"/>
+        <c:crossAx val="-1885680768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-744111040"/>
+        <c:axId val="-1885674256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25.0"/>
@@ -2647,12 +2966,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-743949408"/>
+        <c:crossAx val="-1885670496"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-743949408"/>
+        <c:axId val="-1885670496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2661,7 +2980,834 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-744111040"/>
+        <c:crossAx val="-1885674256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="0"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown Chart For Sprint #4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task Data'!$A$106</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Completed Tasks</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task Data'!$C$106:$P$106</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1885704400"/>
+        <c:axId val="-1885707520"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task Data'!$A$103</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task Data'!$C$103:$P$103</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task Data'!$A$104</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal burndown</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task Data'!$C$104:$P$104</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-1886735152"/>
+        <c:axId val="-1886733104"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task Data'!$A$105</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Tasks Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="42929C"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task Data'!$C$105:$P$105</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-1885704400"/>
+        <c:axId val="-1885707520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1886735152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="&quot;Day&quot;\ \&#10;#0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1886733104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1886733104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Remaining effort</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (hours)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0106619284049409"/>
+              <c:y val="0.363958048275306"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1886735152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1885707520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="30.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Remaining and completed tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.77957124146298"/>
+              <c:y val="0.329852296086731"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1885704400"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="-1885704400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1885707520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2786,6 +3932,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3857,6 +5043,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3916,6 +5618,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>84666</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>148167</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4187,38 +5921,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X66"/>
+  <dimension ref="A1:X106"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="X61" sqref="X61"/>
+    <sheetView topLeftCell="A66" zoomScale="75" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="T103" sqref="T103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="64" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" customWidth="1"/>
     <col min="4" max="23" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="42" x14ac:dyDescent="0.5">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="103"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="121"/>
     </row>
     <row r="2" spans="1:16" ht="35" x14ac:dyDescent="0.35">
       <c r="A2" s="64" t="s">
@@ -5701,31 +7435,31 @@
       </c>
     </row>
     <row r="32" spans="1:23" ht="42" x14ac:dyDescent="0.5">
-      <c r="A32" s="100" t="s">
+      <c r="A32" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="100"/>
-      <c r="C32" s="100"/>
-      <c r="D32" s="100"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="100"/>
-      <c r="G32" s="100"/>
-      <c r="H32" s="100"/>
-      <c r="I32" s="100"/>
-      <c r="J32" s="100"/>
-      <c r="K32" s="100"/>
-      <c r="L32" s="100"/>
-      <c r="M32" s="100"/>
-      <c r="N32" s="100"/>
-      <c r="O32" s="100"/>
-      <c r="P32" s="100"/>
-      <c r="Q32" s="100"/>
-      <c r="R32" s="100"/>
-      <c r="S32" s="100"/>
-      <c r="T32" s="100"/>
-      <c r="U32" s="100"/>
-      <c r="V32" s="100"/>
-      <c r="W32" s="100"/>
+      <c r="B32" s="118"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="118"/>
+      <c r="H32" s="118"/>
+      <c r="I32" s="118"/>
+      <c r="J32" s="118"/>
+      <c r="K32" s="118"/>
+      <c r="L32" s="118"/>
+      <c r="M32" s="118"/>
+      <c r="N32" s="118"/>
+      <c r="O32" s="118"/>
+      <c r="P32" s="118"/>
+      <c r="Q32" s="118"/>
+      <c r="R32" s="118"/>
+      <c r="S32" s="118"/>
+      <c r="T32" s="118"/>
+      <c r="U32" s="118"/>
+      <c r="V32" s="118"/>
+      <c r="W32" s="118"/>
     </row>
     <row r="33" spans="1:23" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="71" t="s">
@@ -7754,14 +9488,1916 @@
       </c>
       <c r="X63" s="77"/>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D66" s="77"/>
-      <c r="E66" s="77"/>
+    <row r="65" spans="1:16" ht="42" x14ac:dyDescent="0.5">
+      <c r="A65" s="122" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="123"/>
+      <c r="C65" s="123"/>
+      <c r="D65" s="123"/>
+      <c r="E65" s="123"/>
+      <c r="F65" s="123"/>
+      <c r="G65" s="123"/>
+      <c r="H65" s="123"/>
+      <c r="I65" s="123"/>
+      <c r="J65" s="123"/>
+      <c r="K65" s="123"/>
+      <c r="L65" s="123"/>
+      <c r="M65" s="123"/>
+      <c r="N65" s="123"/>
+      <c r="O65" s="123"/>
+      <c r="P65" s="124"/>
+    </row>
+    <row r="66" spans="1:16" ht="32" x14ac:dyDescent="0.35">
+      <c r="A66" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="85" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" s="86" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="F66" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="G66" s="86" t="s">
+        <v>30</v>
+      </c>
+      <c r="H66" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="I66" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="J66" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="K66" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="L66" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="M66" s="85" t="s">
+        <v>36</v>
+      </c>
+      <c r="N66" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="O66" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="P66" s="86" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A67" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="83"/>
+      <c r="C67" s="75"/>
+      <c r="D67" s="75"/>
+      <c r="E67" s="75"/>
+      <c r="F67" s="75"/>
+      <c r="G67" s="75"/>
+      <c r="H67" s="75"/>
+      <c r="I67" s="75"/>
+      <c r="J67" s="75"/>
+      <c r="K67" s="75"/>
+      <c r="L67" s="75"/>
+      <c r="M67" s="75"/>
+      <c r="N67" s="75"/>
+      <c r="O67" s="75"/>
+      <c r="P67" s="107"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A68" s="108" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="102">
+        <v>2</v>
+      </c>
+      <c r="C68" s="70">
+        <v>0</v>
+      </c>
+      <c r="D68" s="70">
+        <v>0</v>
+      </c>
+      <c r="E68" s="70">
+        <v>0</v>
+      </c>
+      <c r="F68" s="70">
+        <v>0</v>
+      </c>
+      <c r="G68" s="70">
+        <v>0</v>
+      </c>
+      <c r="H68" s="70">
+        <v>0</v>
+      </c>
+      <c r="I68" s="70">
+        <v>0</v>
+      </c>
+      <c r="J68" s="70">
+        <v>0</v>
+      </c>
+      <c r="K68" s="70">
+        <v>0</v>
+      </c>
+      <c r="L68" s="70">
+        <v>0</v>
+      </c>
+      <c r="M68" s="70">
+        <v>0</v>
+      </c>
+      <c r="N68" s="116">
+        <v>1</v>
+      </c>
+      <c r="O68" s="70">
+        <v>0</v>
+      </c>
+      <c r="P68" s="117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A69" s="108" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" s="102">
+        <v>1</v>
+      </c>
+      <c r="C69" s="70">
+        <v>0</v>
+      </c>
+      <c r="D69" s="70">
+        <v>0</v>
+      </c>
+      <c r="E69" s="70">
+        <v>0</v>
+      </c>
+      <c r="F69" s="70">
+        <v>0</v>
+      </c>
+      <c r="G69" s="70">
+        <v>0</v>
+      </c>
+      <c r="H69" s="70">
+        <v>0</v>
+      </c>
+      <c r="I69" s="70">
+        <v>0</v>
+      </c>
+      <c r="J69" s="70">
+        <v>0</v>
+      </c>
+      <c r="K69" s="70">
+        <v>0</v>
+      </c>
+      <c r="L69" s="70">
+        <v>0</v>
+      </c>
+      <c r="M69" s="70">
+        <v>0</v>
+      </c>
+      <c r="N69" s="116">
+        <v>0.5</v>
+      </c>
+      <c r="O69" s="70">
+        <v>0</v>
+      </c>
+      <c r="P69" s="117">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A70" s="108" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" s="102">
+        <v>0.5</v>
+      </c>
+      <c r="C70" s="70">
+        <v>0</v>
+      </c>
+      <c r="D70" s="70">
+        <v>0</v>
+      </c>
+      <c r="E70" s="70">
+        <v>0</v>
+      </c>
+      <c r="F70" s="70">
+        <v>0</v>
+      </c>
+      <c r="G70" s="70">
+        <v>0</v>
+      </c>
+      <c r="H70" s="70">
+        <v>0</v>
+      </c>
+      <c r="I70" s="70">
+        <v>0</v>
+      </c>
+      <c r="J70" s="70">
+        <v>0</v>
+      </c>
+      <c r="K70" s="70">
+        <v>0</v>
+      </c>
+      <c r="L70" s="70">
+        <v>0</v>
+      </c>
+      <c r="M70" s="70">
+        <v>0</v>
+      </c>
+      <c r="N70" s="70">
+        <v>0</v>
+      </c>
+      <c r="O70" s="70">
+        <v>0</v>
+      </c>
+      <c r="P70" s="117">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A71" s="108" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" s="102">
+        <v>1</v>
+      </c>
+      <c r="C71" s="70">
+        <v>0</v>
+      </c>
+      <c r="D71" s="70">
+        <v>0</v>
+      </c>
+      <c r="E71" s="70">
+        <v>0</v>
+      </c>
+      <c r="F71" s="70">
+        <v>0</v>
+      </c>
+      <c r="G71" s="70">
+        <v>0</v>
+      </c>
+      <c r="H71" s="70">
+        <v>0</v>
+      </c>
+      <c r="I71" s="70">
+        <v>0</v>
+      </c>
+      <c r="J71" s="70">
+        <v>0</v>
+      </c>
+      <c r="K71" s="70">
+        <v>0</v>
+      </c>
+      <c r="L71" s="70">
+        <v>0</v>
+      </c>
+      <c r="M71" s="70">
+        <v>0</v>
+      </c>
+      <c r="N71" s="70">
+        <v>0</v>
+      </c>
+      <c r="O71" s="70">
+        <v>0</v>
+      </c>
+      <c r="P71" s="117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A72" s="106" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" s="83"/>
+      <c r="C72" s="75"/>
+      <c r="D72" s="75"/>
+      <c r="E72" s="75"/>
+      <c r="F72" s="75"/>
+      <c r="G72" s="75"/>
+      <c r="H72" s="75"/>
+      <c r="I72" s="75"/>
+      <c r="J72" s="75"/>
+      <c r="K72" s="75"/>
+      <c r="L72" s="75"/>
+      <c r="M72" s="75"/>
+      <c r="N72" s="75"/>
+      <c r="O72" s="75"/>
+      <c r="P72" s="107"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A73" s="108" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" s="102">
+        <v>3</v>
+      </c>
+      <c r="C73" s="70">
+        <v>0</v>
+      </c>
+      <c r="D73" s="70">
+        <v>0</v>
+      </c>
+      <c r="E73" s="70">
+        <v>0</v>
+      </c>
+      <c r="F73" s="70">
+        <v>0</v>
+      </c>
+      <c r="G73" s="70">
+        <v>0</v>
+      </c>
+      <c r="H73" s="70">
+        <v>0</v>
+      </c>
+      <c r="I73" s="70">
+        <v>0</v>
+      </c>
+      <c r="J73" s="70">
+        <v>0</v>
+      </c>
+      <c r="K73" s="70">
+        <v>0</v>
+      </c>
+      <c r="L73" s="70">
+        <v>0</v>
+      </c>
+      <c r="M73" s="70">
+        <v>0</v>
+      </c>
+      <c r="N73" s="70">
+        <v>0</v>
+      </c>
+      <c r="O73" s="70">
+        <v>0</v>
+      </c>
+      <c r="P73" s="117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A74" s="108" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" s="102">
+        <v>2</v>
+      </c>
+      <c r="C74" s="70">
+        <v>0</v>
+      </c>
+      <c r="D74" s="70">
+        <v>0</v>
+      </c>
+      <c r="E74" s="70">
+        <v>0</v>
+      </c>
+      <c r="F74" s="70">
+        <v>0</v>
+      </c>
+      <c r="G74" s="70">
+        <v>0</v>
+      </c>
+      <c r="H74" s="70">
+        <v>0</v>
+      </c>
+      <c r="I74" s="70">
+        <v>0</v>
+      </c>
+      <c r="J74" s="70">
+        <v>0</v>
+      </c>
+      <c r="K74" s="70">
+        <v>0</v>
+      </c>
+      <c r="L74" s="70">
+        <v>0</v>
+      </c>
+      <c r="M74" s="70">
+        <v>0</v>
+      </c>
+      <c r="N74" s="70">
+        <v>0</v>
+      </c>
+      <c r="O74" s="70">
+        <v>0</v>
+      </c>
+      <c r="P74" s="117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A75" s="108" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" s="102">
+        <v>1</v>
+      </c>
+      <c r="C75" s="70">
+        <v>0</v>
+      </c>
+      <c r="D75" s="70">
+        <v>0</v>
+      </c>
+      <c r="E75" s="70">
+        <v>0</v>
+      </c>
+      <c r="F75" s="70">
+        <v>0</v>
+      </c>
+      <c r="G75" s="70">
+        <v>0</v>
+      </c>
+      <c r="H75" s="70">
+        <v>0</v>
+      </c>
+      <c r="I75" s="70">
+        <v>0</v>
+      </c>
+      <c r="J75" s="70">
+        <v>0</v>
+      </c>
+      <c r="K75" s="70">
+        <v>0</v>
+      </c>
+      <c r="L75" s="70">
+        <v>0</v>
+      </c>
+      <c r="M75" s="70">
+        <v>0</v>
+      </c>
+      <c r="N75" s="70">
+        <v>0</v>
+      </c>
+      <c r="O75" s="70">
+        <v>0</v>
+      </c>
+      <c r="P75" s="117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A76" s="108" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" s="102">
+        <v>1</v>
+      </c>
+      <c r="C76" s="70">
+        <v>0</v>
+      </c>
+      <c r="D76" s="70">
+        <v>0</v>
+      </c>
+      <c r="E76" s="70">
+        <v>0</v>
+      </c>
+      <c r="F76" s="70">
+        <v>0</v>
+      </c>
+      <c r="G76" s="70">
+        <v>0</v>
+      </c>
+      <c r="H76" s="70">
+        <v>0</v>
+      </c>
+      <c r="I76" s="70">
+        <v>0</v>
+      </c>
+      <c r="J76" s="70">
+        <v>0</v>
+      </c>
+      <c r="K76" s="70">
+        <v>0</v>
+      </c>
+      <c r="L76" s="70">
+        <v>0</v>
+      </c>
+      <c r="M76" s="70">
+        <v>0</v>
+      </c>
+      <c r="N76" s="70">
+        <v>0</v>
+      </c>
+      <c r="O76" s="70">
+        <v>0</v>
+      </c>
+      <c r="P76" s="117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A77" s="106" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" s="83"/>
+      <c r="C77" s="75"/>
+      <c r="D77" s="75"/>
+      <c r="E77" s="75"/>
+      <c r="F77" s="75"/>
+      <c r="G77" s="75"/>
+      <c r="H77" s="75"/>
+      <c r="I77" s="75"/>
+      <c r="J77" s="75"/>
+      <c r="K77" s="75"/>
+      <c r="L77" s="75"/>
+      <c r="M77" s="75"/>
+      <c r="N77" s="75"/>
+      <c r="O77" s="75"/>
+      <c r="P77" s="107"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A78" s="108" t="s">
+        <v>88</v>
+      </c>
+      <c r="B78" s="102">
+        <v>1</v>
+      </c>
+      <c r="C78" s="70">
+        <v>0</v>
+      </c>
+      <c r="D78" s="70">
+        <v>0</v>
+      </c>
+      <c r="E78" s="70">
+        <v>0</v>
+      </c>
+      <c r="F78" s="70">
+        <v>0</v>
+      </c>
+      <c r="G78" s="117">
+        <v>1</v>
+      </c>
+      <c r="H78" s="70">
+        <v>0</v>
+      </c>
+      <c r="I78" s="70">
+        <v>0</v>
+      </c>
+      <c r="J78" s="70">
+        <v>0</v>
+      </c>
+      <c r="K78" s="70">
+        <v>0</v>
+      </c>
+      <c r="L78" s="70">
+        <v>0</v>
+      </c>
+      <c r="M78" s="70">
+        <v>0</v>
+      </c>
+      <c r="N78" s="70">
+        <v>0</v>
+      </c>
+      <c r="O78" s="70">
+        <v>0</v>
+      </c>
+      <c r="P78" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A79" s="108" t="s">
+        <v>89</v>
+      </c>
+      <c r="B79" s="102">
+        <v>1</v>
+      </c>
+      <c r="C79" s="70">
+        <v>0</v>
+      </c>
+      <c r="D79" s="70">
+        <v>0</v>
+      </c>
+      <c r="E79" s="70">
+        <v>0</v>
+      </c>
+      <c r="F79" s="70">
+        <v>0</v>
+      </c>
+      <c r="G79" s="117">
+        <v>1</v>
+      </c>
+      <c r="H79" s="70">
+        <v>0</v>
+      </c>
+      <c r="I79" s="70">
+        <v>0</v>
+      </c>
+      <c r="J79" s="70">
+        <v>0</v>
+      </c>
+      <c r="K79" s="70">
+        <v>0</v>
+      </c>
+      <c r="L79" s="70">
+        <v>0</v>
+      </c>
+      <c r="M79" s="70">
+        <v>0</v>
+      </c>
+      <c r="N79" s="70">
+        <v>0</v>
+      </c>
+      <c r="O79" s="70">
+        <v>0</v>
+      </c>
+      <c r="P79" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A80" s="108" t="s">
+        <v>90</v>
+      </c>
+      <c r="B80" s="102">
+        <v>0.5</v>
+      </c>
+      <c r="C80" s="70">
+        <v>0</v>
+      </c>
+      <c r="D80" s="70">
+        <v>0</v>
+      </c>
+      <c r="E80" s="70">
+        <v>0</v>
+      </c>
+      <c r="F80" s="70">
+        <v>0</v>
+      </c>
+      <c r="G80" s="70">
+        <v>0</v>
+      </c>
+      <c r="H80" s="70">
+        <v>0</v>
+      </c>
+      <c r="I80" s="70">
+        <v>0</v>
+      </c>
+      <c r="J80" s="70">
+        <v>0</v>
+      </c>
+      <c r="K80" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="L80" s="70">
+        <v>0</v>
+      </c>
+      <c r="M80" s="70">
+        <v>0</v>
+      </c>
+      <c r="N80" s="70">
+        <v>0</v>
+      </c>
+      <c r="O80" s="70">
+        <v>0</v>
+      </c>
+      <c r="P80" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A81" s="108" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" s="102">
+        <v>0.5</v>
+      </c>
+      <c r="C81" s="70">
+        <v>0</v>
+      </c>
+      <c r="D81" s="70">
+        <v>0</v>
+      </c>
+      <c r="E81" s="70">
+        <v>0</v>
+      </c>
+      <c r="F81" s="70">
+        <v>0</v>
+      </c>
+      <c r="G81" s="70">
+        <v>0</v>
+      </c>
+      <c r="H81" s="70">
+        <v>0</v>
+      </c>
+      <c r="I81" s="70">
+        <v>0</v>
+      </c>
+      <c r="J81" s="70">
+        <v>0</v>
+      </c>
+      <c r="K81" s="70">
+        <v>0</v>
+      </c>
+      <c r="L81" s="70">
+        <v>0</v>
+      </c>
+      <c r="M81" s="70">
+        <v>0</v>
+      </c>
+      <c r="N81" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="O81" s="70">
+        <v>0</v>
+      </c>
+      <c r="P81" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A82" s="108" t="s">
+        <v>92</v>
+      </c>
+      <c r="B82" s="102">
+        <v>0.5</v>
+      </c>
+      <c r="C82" s="70">
+        <v>0</v>
+      </c>
+      <c r="D82" s="70">
+        <v>0</v>
+      </c>
+      <c r="E82" s="70">
+        <v>0</v>
+      </c>
+      <c r="F82" s="70">
+        <v>0</v>
+      </c>
+      <c r="G82" s="70">
+        <v>0</v>
+      </c>
+      <c r="H82" s="70">
+        <v>0</v>
+      </c>
+      <c r="I82" s="70">
+        <v>0</v>
+      </c>
+      <c r="J82" s="70">
+        <v>0</v>
+      </c>
+      <c r="K82" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="L82" s="70">
+        <v>0</v>
+      </c>
+      <c r="M82" s="70">
+        <v>0</v>
+      </c>
+      <c r="N82" s="70">
+        <v>0</v>
+      </c>
+      <c r="O82" s="70">
+        <v>0</v>
+      </c>
+      <c r="P82" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A83" s="106" t="s">
+        <v>106</v>
+      </c>
+      <c r="B83" s="83"/>
+      <c r="C83" s="75"/>
+      <c r="D83" s="75"/>
+      <c r="E83" s="75"/>
+      <c r="F83" s="75"/>
+      <c r="G83" s="75"/>
+      <c r="H83" s="75"/>
+      <c r="I83" s="75"/>
+      <c r="J83" s="75"/>
+      <c r="K83" s="75"/>
+      <c r="L83" s="75"/>
+      <c r="M83" s="75"/>
+      <c r="N83" s="75"/>
+      <c r="O83" s="75"/>
+      <c r="P83" s="107"/>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A84" s="108" t="s">
+        <v>107</v>
+      </c>
+      <c r="B84" s="102">
+        <v>1</v>
+      </c>
+      <c r="C84" s="70">
+        <v>0</v>
+      </c>
+      <c r="D84" s="70">
+        <v>0</v>
+      </c>
+      <c r="E84" s="70">
+        <v>0</v>
+      </c>
+      <c r="F84" s="70">
+        <v>0</v>
+      </c>
+      <c r="G84" s="70">
+        <v>0</v>
+      </c>
+      <c r="H84" s="70">
+        <v>0</v>
+      </c>
+      <c r="I84" s="117">
+        <v>1</v>
+      </c>
+      <c r="J84" s="70">
+        <v>0</v>
+      </c>
+      <c r="K84" s="70">
+        <v>0</v>
+      </c>
+      <c r="L84" s="70">
+        <v>0</v>
+      </c>
+      <c r="M84" s="70">
+        <v>0</v>
+      </c>
+      <c r="N84" s="70">
+        <v>0</v>
+      </c>
+      <c r="O84" s="70">
+        <v>0</v>
+      </c>
+      <c r="P84" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A85" s="108" t="s">
+        <v>108</v>
+      </c>
+      <c r="B85" s="102">
+        <v>1</v>
+      </c>
+      <c r="C85" s="70">
+        <v>0</v>
+      </c>
+      <c r="D85" s="70">
+        <v>0</v>
+      </c>
+      <c r="E85" s="70">
+        <v>0</v>
+      </c>
+      <c r="F85" s="70">
+        <v>0</v>
+      </c>
+      <c r="G85" s="70">
+        <v>0</v>
+      </c>
+      <c r="H85" s="70">
+        <v>0</v>
+      </c>
+      <c r="I85" s="117">
+        <v>1</v>
+      </c>
+      <c r="J85" s="70">
+        <v>0</v>
+      </c>
+      <c r="K85" s="70">
+        <v>0</v>
+      </c>
+      <c r="L85" s="70">
+        <v>0</v>
+      </c>
+      <c r="M85" s="70">
+        <v>0</v>
+      </c>
+      <c r="N85" s="70">
+        <v>0</v>
+      </c>
+      <c r="O85" s="70">
+        <v>0</v>
+      </c>
+      <c r="P85" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A86" s="108" t="s">
+        <v>109</v>
+      </c>
+      <c r="B86" s="102">
+        <v>0.5</v>
+      </c>
+      <c r="C86" s="70">
+        <v>0</v>
+      </c>
+      <c r="D86" s="70">
+        <v>0</v>
+      </c>
+      <c r="E86" s="70">
+        <v>0</v>
+      </c>
+      <c r="F86" s="70">
+        <v>0</v>
+      </c>
+      <c r="G86" s="70">
+        <v>0</v>
+      </c>
+      <c r="H86" s="70">
+        <v>0</v>
+      </c>
+      <c r="I86" s="70">
+        <v>0</v>
+      </c>
+      <c r="J86" s="70">
+        <v>0</v>
+      </c>
+      <c r="K86" s="70">
+        <v>0</v>
+      </c>
+      <c r="L86" s="70">
+        <v>0</v>
+      </c>
+      <c r="M86" s="70">
+        <v>0</v>
+      </c>
+      <c r="N86" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="O86" s="70">
+        <v>0</v>
+      </c>
+      <c r="P86" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A87" s="108" t="s">
+        <v>110</v>
+      </c>
+      <c r="B87" s="102">
+        <v>0.5</v>
+      </c>
+      <c r="C87" s="70">
+        <v>0</v>
+      </c>
+      <c r="D87" s="70">
+        <v>0</v>
+      </c>
+      <c r="E87" s="70">
+        <v>0</v>
+      </c>
+      <c r="F87" s="70">
+        <v>0</v>
+      </c>
+      <c r="G87" s="70">
+        <v>0</v>
+      </c>
+      <c r="H87" s="70">
+        <v>0</v>
+      </c>
+      <c r="I87" s="70">
+        <v>0</v>
+      </c>
+      <c r="J87" s="70">
+        <v>0</v>
+      </c>
+      <c r="K87" s="70">
+        <v>0</v>
+      </c>
+      <c r="L87" s="70">
+        <v>0</v>
+      </c>
+      <c r="M87" s="70">
+        <v>0</v>
+      </c>
+      <c r="N87" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="O87" s="70">
+        <v>0</v>
+      </c>
+      <c r="P87" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A88" s="106" t="s">
+        <v>78</v>
+      </c>
+      <c r="B88" s="83"/>
+      <c r="C88" s="75"/>
+      <c r="D88" s="75"/>
+      <c r="E88" s="75"/>
+      <c r="F88" s="75"/>
+      <c r="G88" s="75"/>
+      <c r="H88" s="75"/>
+      <c r="I88" s="75"/>
+      <c r="J88" s="75"/>
+      <c r="K88" s="75"/>
+      <c r="L88" s="75"/>
+      <c r="M88" s="75"/>
+      <c r="N88" s="75"/>
+      <c r="O88" s="75"/>
+      <c r="P88" s="107"/>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A89" s="108" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" s="101">
+        <v>1</v>
+      </c>
+      <c r="C89" s="70">
+        <v>0</v>
+      </c>
+      <c r="D89" s="70">
+        <v>0</v>
+      </c>
+      <c r="E89" s="70">
+        <v>0</v>
+      </c>
+      <c r="F89" s="70">
+        <v>0</v>
+      </c>
+      <c r="G89" s="117">
+        <v>1</v>
+      </c>
+      <c r="H89" s="70">
+        <v>0</v>
+      </c>
+      <c r="I89" s="70">
+        <v>0</v>
+      </c>
+      <c r="J89" s="70">
+        <v>0</v>
+      </c>
+      <c r="K89" s="70">
+        <v>0</v>
+      </c>
+      <c r="L89" s="70">
+        <v>0</v>
+      </c>
+      <c r="M89" s="70">
+        <v>0</v>
+      </c>
+      <c r="N89" s="70">
+        <v>0</v>
+      </c>
+      <c r="O89" s="70">
+        <v>0</v>
+      </c>
+      <c r="P89" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A90" s="108" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" s="102">
+        <v>3</v>
+      </c>
+      <c r="C90" s="70">
+        <v>0</v>
+      </c>
+      <c r="D90" s="70">
+        <v>0</v>
+      </c>
+      <c r="E90" s="70">
+        <v>0</v>
+      </c>
+      <c r="F90" s="70">
+        <v>0</v>
+      </c>
+      <c r="G90" s="116">
+        <v>0.5</v>
+      </c>
+      <c r="H90" s="70">
+        <v>0</v>
+      </c>
+      <c r="I90" s="70">
+        <v>0</v>
+      </c>
+      <c r="J90" s="70">
+        <v>0</v>
+      </c>
+      <c r="K90" s="116">
+        <v>2</v>
+      </c>
+      <c r="L90" s="70">
+        <v>0</v>
+      </c>
+      <c r="M90" s="70">
+        <v>0</v>
+      </c>
+      <c r="N90" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="O90" s="70">
+        <v>0</v>
+      </c>
+      <c r="P90" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A91" s="108" t="s">
+        <v>95</v>
+      </c>
+      <c r="B91" s="102">
+        <v>2</v>
+      </c>
+      <c r="C91" s="70">
+        <v>0</v>
+      </c>
+      <c r="D91" s="70">
+        <v>0</v>
+      </c>
+      <c r="E91" s="70">
+        <v>0</v>
+      </c>
+      <c r="F91" s="70">
+        <v>0</v>
+      </c>
+      <c r="G91" s="70">
+        <v>0</v>
+      </c>
+      <c r="H91" s="70">
+        <v>0</v>
+      </c>
+      <c r="I91" s="70">
+        <v>0</v>
+      </c>
+      <c r="J91" s="70">
+        <v>0</v>
+      </c>
+      <c r="K91" s="116">
+        <v>1</v>
+      </c>
+      <c r="L91" s="70">
+        <v>0</v>
+      </c>
+      <c r="M91" s="70">
+        <v>0</v>
+      </c>
+      <c r="N91" s="117">
+        <v>1</v>
+      </c>
+      <c r="O91" s="70">
+        <v>0</v>
+      </c>
+      <c r="P91" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A92" s="108" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="102">
+        <v>2</v>
+      </c>
+      <c r="C92" s="70">
+        <v>0</v>
+      </c>
+      <c r="D92" s="70">
+        <v>0</v>
+      </c>
+      <c r="E92" s="70">
+        <v>0</v>
+      </c>
+      <c r="F92" s="70">
+        <v>0</v>
+      </c>
+      <c r="G92" s="70">
+        <v>0</v>
+      </c>
+      <c r="H92" s="70">
+        <v>0</v>
+      </c>
+      <c r="I92" s="70">
+        <v>0</v>
+      </c>
+      <c r="J92" s="70">
+        <v>0</v>
+      </c>
+      <c r="K92" s="70">
+        <v>0</v>
+      </c>
+      <c r="L92" s="70">
+        <v>0</v>
+      </c>
+      <c r="M92" s="70">
+        <v>0</v>
+      </c>
+      <c r="N92" s="117">
+        <v>2</v>
+      </c>
+      <c r="O92" s="70">
+        <v>0</v>
+      </c>
+      <c r="P92" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A93" s="108" t="s">
+        <v>97</v>
+      </c>
+      <c r="B93" s="102">
+        <v>1</v>
+      </c>
+      <c r="C93" s="70">
+        <v>0</v>
+      </c>
+      <c r="D93" s="70">
+        <v>0</v>
+      </c>
+      <c r="E93" s="70">
+        <v>0</v>
+      </c>
+      <c r="F93" s="70">
+        <v>0</v>
+      </c>
+      <c r="G93" s="70">
+        <v>0</v>
+      </c>
+      <c r="H93" s="70">
+        <v>0</v>
+      </c>
+      <c r="I93" s="70">
+        <v>0</v>
+      </c>
+      <c r="J93" s="70">
+        <v>0</v>
+      </c>
+      <c r="K93" s="70">
+        <v>0</v>
+      </c>
+      <c r="L93" s="70">
+        <v>0</v>
+      </c>
+      <c r="M93" s="70">
+        <v>0</v>
+      </c>
+      <c r="N93" s="117">
+        <v>1</v>
+      </c>
+      <c r="O93" s="70">
+        <v>0</v>
+      </c>
+      <c r="P93" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A94" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" s="83"/>
+      <c r="C94" s="75"/>
+      <c r="D94" s="75"/>
+      <c r="E94" s="75"/>
+      <c r="F94" s="75"/>
+      <c r="G94" s="75"/>
+      <c r="H94" s="75"/>
+      <c r="I94" s="75"/>
+      <c r="J94" s="75"/>
+      <c r="K94" s="75"/>
+      <c r="L94" s="75"/>
+      <c r="M94" s="75"/>
+      <c r="N94" s="75"/>
+      <c r="O94" s="75"/>
+      <c r="P94" s="107"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A95" s="108" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" s="101">
+        <v>1</v>
+      </c>
+      <c r="C95" s="70">
+        <v>0</v>
+      </c>
+      <c r="D95" s="70">
+        <v>0</v>
+      </c>
+      <c r="E95" s="70">
+        <v>0</v>
+      </c>
+      <c r="F95" s="70">
+        <v>0</v>
+      </c>
+      <c r="G95" s="70">
+        <v>0</v>
+      </c>
+      <c r="H95" s="70">
+        <v>0</v>
+      </c>
+      <c r="I95" s="117">
+        <v>1</v>
+      </c>
+      <c r="J95" s="70">
+        <v>0</v>
+      </c>
+      <c r="K95" s="70">
+        <v>0</v>
+      </c>
+      <c r="L95" s="70">
+        <v>0</v>
+      </c>
+      <c r="M95" s="70">
+        <v>0</v>
+      </c>
+      <c r="N95" s="70">
+        <v>0</v>
+      </c>
+      <c r="O95" s="70">
+        <v>0</v>
+      </c>
+      <c r="P95" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A96" s="109" t="s">
+        <v>99</v>
+      </c>
+      <c r="B96" s="100">
+        <v>2</v>
+      </c>
+      <c r="C96" s="70">
+        <v>0</v>
+      </c>
+      <c r="D96" s="70">
+        <v>0</v>
+      </c>
+      <c r="E96" s="70">
+        <v>0</v>
+      </c>
+      <c r="F96" s="70">
+        <v>0</v>
+      </c>
+      <c r="G96" s="70">
+        <v>0</v>
+      </c>
+      <c r="H96" s="70">
+        <v>0</v>
+      </c>
+      <c r="I96" s="116">
+        <v>1</v>
+      </c>
+      <c r="J96" s="70">
+        <v>0</v>
+      </c>
+      <c r="K96" s="70">
+        <v>0</v>
+      </c>
+      <c r="L96" s="70">
+        <v>0</v>
+      </c>
+      <c r="M96" s="70">
+        <v>0</v>
+      </c>
+      <c r="N96" s="117">
+        <v>1</v>
+      </c>
+      <c r="O96" s="70">
+        <v>0</v>
+      </c>
+      <c r="P96" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A97" s="110" t="s">
+        <v>80</v>
+      </c>
+      <c r="B97" s="104"/>
+      <c r="C97" s="105"/>
+      <c r="D97" s="105"/>
+      <c r="E97" s="105"/>
+      <c r="F97" s="105"/>
+      <c r="G97" s="105"/>
+      <c r="H97" s="105"/>
+      <c r="I97" s="105"/>
+      <c r="J97" s="105"/>
+      <c r="K97" s="105"/>
+      <c r="L97" s="105"/>
+      <c r="M97" s="105"/>
+      <c r="N97" s="105"/>
+      <c r="O97" s="105"/>
+      <c r="P97" s="111"/>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A98" s="112" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" s="103">
+        <v>1</v>
+      </c>
+      <c r="C98" s="70">
+        <v>0</v>
+      </c>
+      <c r="D98" s="70">
+        <v>0</v>
+      </c>
+      <c r="E98" s="70">
+        <v>0</v>
+      </c>
+      <c r="F98" s="70">
+        <v>0</v>
+      </c>
+      <c r="G98" s="70">
+        <v>0</v>
+      </c>
+      <c r="H98" s="70">
+        <v>0</v>
+      </c>
+      <c r="I98" s="70">
+        <v>0</v>
+      </c>
+      <c r="J98" s="70">
+        <v>0</v>
+      </c>
+      <c r="K98" s="70">
+        <v>0</v>
+      </c>
+      <c r="L98" s="70">
+        <v>0</v>
+      </c>
+      <c r="M98" s="70">
+        <v>0</v>
+      </c>
+      <c r="N98" s="117">
+        <v>1</v>
+      </c>
+      <c r="O98" s="70">
+        <v>0</v>
+      </c>
+      <c r="P98" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A99" s="108" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" s="102">
+        <v>1</v>
+      </c>
+      <c r="C99" s="70">
+        <v>0</v>
+      </c>
+      <c r="D99" s="70">
+        <v>0</v>
+      </c>
+      <c r="E99" s="70">
+        <v>0</v>
+      </c>
+      <c r="F99" s="70">
+        <v>0</v>
+      </c>
+      <c r="G99" s="70">
+        <v>0</v>
+      </c>
+      <c r="H99" s="70">
+        <v>0</v>
+      </c>
+      <c r="I99" s="116">
+        <v>0.5</v>
+      </c>
+      <c r="J99" s="70">
+        <v>0</v>
+      </c>
+      <c r="K99" s="70">
+        <v>0</v>
+      </c>
+      <c r="L99" s="70">
+        <v>0</v>
+      </c>
+      <c r="M99" s="70">
+        <v>0</v>
+      </c>
+      <c r="N99" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="O99" s="70">
+        <v>0</v>
+      </c>
+      <c r="P99" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A100" s="108" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" s="102">
+        <v>1</v>
+      </c>
+      <c r="C100" s="70">
+        <v>0</v>
+      </c>
+      <c r="D100" s="70">
+        <v>0</v>
+      </c>
+      <c r="E100" s="70">
+        <v>0</v>
+      </c>
+      <c r="F100" s="70">
+        <v>0</v>
+      </c>
+      <c r="G100" s="117">
+        <v>1</v>
+      </c>
+      <c r="H100" s="70">
+        <v>0</v>
+      </c>
+      <c r="I100" s="70">
+        <v>0</v>
+      </c>
+      <c r="J100" s="70">
+        <v>0</v>
+      </c>
+      <c r="K100" s="70">
+        <v>0</v>
+      </c>
+      <c r="L100" s="70">
+        <v>0</v>
+      </c>
+      <c r="M100" s="70">
+        <v>0</v>
+      </c>
+      <c r="N100" s="70">
+        <v>0</v>
+      </c>
+      <c r="O100" s="70">
+        <v>0</v>
+      </c>
+      <c r="P100" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A101" s="108" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" s="102">
+        <v>1</v>
+      </c>
+      <c r="C101" s="70">
+        <v>0</v>
+      </c>
+      <c r="D101" s="70">
+        <v>0</v>
+      </c>
+      <c r="E101" s="70">
+        <v>0</v>
+      </c>
+      <c r="F101" s="70">
+        <v>0</v>
+      </c>
+      <c r="G101" s="70">
+        <v>0</v>
+      </c>
+      <c r="H101" s="70">
+        <v>0</v>
+      </c>
+      <c r="I101" s="116">
+        <v>0.5</v>
+      </c>
+      <c r="J101" s="70">
+        <v>0</v>
+      </c>
+      <c r="K101" s="70">
+        <v>0</v>
+      </c>
+      <c r="L101" s="70">
+        <v>0</v>
+      </c>
+      <c r="M101" s="70">
+        <v>0</v>
+      </c>
+      <c r="N101" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="O101" s="70">
+        <v>0</v>
+      </c>
+      <c r="P101" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A102" s="108" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" s="102">
+        <v>1</v>
+      </c>
+      <c r="C102" s="70">
+        <v>0</v>
+      </c>
+      <c r="D102" s="70">
+        <v>0</v>
+      </c>
+      <c r="E102" s="70">
+        <v>0</v>
+      </c>
+      <c r="F102" s="70">
+        <v>0</v>
+      </c>
+      <c r="G102" s="70">
+        <v>0</v>
+      </c>
+      <c r="H102" s="70">
+        <v>0</v>
+      </c>
+      <c r="I102" s="70">
+        <v>0</v>
+      </c>
+      <c r="J102" s="70">
+        <v>0</v>
+      </c>
+      <c r="K102" s="70">
+        <v>0</v>
+      </c>
+      <c r="L102" s="70">
+        <v>0</v>
+      </c>
+      <c r="M102" s="70">
+        <v>0</v>
+      </c>
+      <c r="N102" s="117">
+        <v>1</v>
+      </c>
+      <c r="O102" s="70">
+        <v>0</v>
+      </c>
+      <c r="P102" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A103" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B103" s="78">
+        <f>SUM(B67:B102)</f>
+        <v>35</v>
+      </c>
+      <c r="C103" s="32">
+        <f t="shared" ref="C103:P103" si="4">SUM(B103-SUM(C67:C102))</f>
+        <v>35</v>
+      </c>
+      <c r="D103" s="32">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="E103" s="32">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="F103" s="32">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="G103" s="32">
+        <f t="shared" si="4"/>
+        <v>30.5</v>
+      </c>
+      <c r="H103" s="32">
+        <f t="shared" si="4"/>
+        <v>30.5</v>
+      </c>
+      <c r="I103" s="32">
+        <f t="shared" si="4"/>
+        <v>25.5</v>
+      </c>
+      <c r="J103" s="32">
+        <f t="shared" si="4"/>
+        <v>25.5</v>
+      </c>
+      <c r="K103" s="32">
+        <f t="shared" si="4"/>
+        <v>21.5</v>
+      </c>
+      <c r="L103" s="32">
+        <f t="shared" si="4"/>
+        <v>21.5</v>
+      </c>
+      <c r="M103" s="32">
+        <f t="shared" si="4"/>
+        <v>21.5</v>
+      </c>
+      <c r="N103" s="32">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="O103" s="32">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="P103" s="32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A104" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B104" s="79">
+        <f>B103</f>
+        <v>35</v>
+      </c>
+      <c r="C104" s="6">
+        <f>B104-$B104/COLUMNS(C66:P66)</f>
+        <v>32.5</v>
+      </c>
+      <c r="D104" s="6">
+        <f>C104-$B104/COLUMNS(D66:Q66)</f>
+        <v>30</v>
+      </c>
+      <c r="E104" s="6">
+        <f t="shared" ref="E104:P104" si="5">D104-$B104/COLUMNS(E66:R66)</f>
+        <v>27.5</v>
+      </c>
+      <c r="F104" s="6">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="G104" s="6">
+        <f t="shared" si="5"/>
+        <v>22.5</v>
+      </c>
+      <c r="H104" s="6">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I104" s="6">
+        <f t="shared" si="5"/>
+        <v>17.5</v>
+      </c>
+      <c r="J104" s="6">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="K104" s="6">
+        <f t="shared" si="5"/>
+        <v>12.5</v>
+      </c>
+      <c r="L104" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="M104" s="6">
+        <f t="shared" si="5"/>
+        <v>7.5</v>
+      </c>
+      <c r="N104" s="6">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="O104" s="6">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="P104" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A105" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B105" s="50">
+        <f>COUNTIF(B67:B102, "&gt;0")</f>
+        <v>29</v>
+      </c>
+      <c r="C105" s="50">
+        <f>B105-C106</f>
+        <v>29</v>
+      </c>
+      <c r="D105" s="50">
+        <f>C105-D106</f>
+        <v>29</v>
+      </c>
+      <c r="E105" s="50">
+        <f>D105-E106</f>
+        <v>29</v>
+      </c>
+      <c r="F105" s="50">
+        <f t="shared" ref="F105:P105" si="6">E105-F106</f>
+        <v>29</v>
+      </c>
+      <c r="G105" s="50">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="H105" s="50">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="I105" s="50">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+      <c r="J105" s="50">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+      <c r="K105" s="50">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="L105" s="50">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="M105" s="50">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="N105" s="50">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="O105" s="50">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P105" s="50">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A106" s="113" t="s">
+        <v>43</v>
+      </c>
+      <c r="B106" s="114">
+        <v>0</v>
+      </c>
+      <c r="C106" s="114">
+        <v>0</v>
+      </c>
+      <c r="D106" s="114">
+        <v>0</v>
+      </c>
+      <c r="E106" s="114">
+        <v>0</v>
+      </c>
+      <c r="F106" s="114">
+        <v>0</v>
+      </c>
+      <c r="G106" s="114">
+        <v>4</v>
+      </c>
+      <c r="H106" s="114">
+        <v>0</v>
+      </c>
+      <c r="I106" s="114">
+        <v>3</v>
+      </c>
+      <c r="J106" s="114">
+        <v>0</v>
+      </c>
+      <c r="K106" s="114">
+        <v>2</v>
+      </c>
+      <c r="L106" s="114">
+        <v>0</v>
+      </c>
+      <c r="M106" s="114">
+        <v>0</v>
+      </c>
+      <c r="N106" s="114">
+        <v>12</v>
+      </c>
+      <c r="O106" s="114">
+        <v>0</v>
+      </c>
+      <c r="P106" s="115">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A32:W32"/>
     <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A65:P65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7771,8 +11407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="AB11" sqref="AB11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
refactored unit tests referenced github issue for every unit test
</commit_message>
<xml_diff>
--- a/Documentation/BurndownChart.xlsx
+++ b/Documentation/BurndownChart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="44420" yWindow="2940" windowWidth="32280" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="43100" yWindow="440" windowWidth="33620" windowHeight="28360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Task Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="128">
   <si>
     <t>Create the login/signup page</t>
   </si>
@@ -361,6 +361,57 @@
   </si>
   <si>
     <t>Create http request to load biography from server</t>
+  </si>
+  <si>
+    <t>SPRINT 5</t>
+  </si>
+  <si>
+    <t>US-21: Delete a Joined Course from Profile (6)</t>
+  </si>
+  <si>
+    <t>Add a delete function to the courses route.</t>
+  </si>
+  <si>
+    <t>Add a button in the view to leave a course you are a member of.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connect the route to the view. </t>
+  </si>
+  <si>
+    <t>US-22: Rename Uploaded Documents (7)</t>
+  </si>
+  <si>
+    <t>Create an api end route to update the document name</t>
+  </si>
+  <si>
+    <t>Build the form on the front end to edit the name</t>
+  </si>
+  <si>
+    <t>Connect the view to the route</t>
+  </si>
+  <si>
+    <t>Decide on the external service to use</t>
+  </si>
+  <si>
+    <t>Integrate the external service into the application</t>
+  </si>
+  <si>
+    <t>Send the notification</t>
+  </si>
+  <si>
+    <t>US-AC: Unit Testing (10)</t>
+  </si>
+  <si>
+    <t>unit tests</t>
+  </si>
+  <si>
+    <t>keeping track of all the meeting minutes and slack conversations</t>
+  </si>
+  <si>
+    <t>US-AB: Documentation (10)</t>
+  </si>
+  <si>
+    <t>US-06: New Document Notifications (9)</t>
   </si>
 </sst>
 </file>
@@ -1311,8 +1362,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FF42929C"/>
       <color rgb="FFD882BF"/>
-      <color rgb="FF42929C"/>
       <color rgb="FFFF86FA"/>
     </mruColors>
   </colors>
@@ -1486,8 +1537,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1886781392"/>
-        <c:axId val="-1886785600"/>
+        <c:axId val="2091276256"/>
+        <c:axId val="2091272864"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1680,8 +1731,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1885721792"/>
-        <c:axId val="-1885719472"/>
+        <c:axId val="2090032464"/>
+        <c:axId val="2090054144"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1775,11 +1826,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1886781392"/>
-        <c:axId val="-1886785600"/>
+        <c:axId val="2091276256"/>
+        <c:axId val="2091272864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1885721792"/>
+        <c:axId val="2090032464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1822,7 +1873,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885719472"/>
+        <c:crossAx val="2090054144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1830,7 +1881,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1885719472"/>
+        <c:axId val="2090054144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1950,12 +2001,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885721792"/>
+        <c:crossAx val="2090032464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1886785600"/>
+        <c:axId val="2091272864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25.0"/>
@@ -2056,12 +2107,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1886781392"/>
+        <c:crossAx val="2091276256"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1886781392"/>
+        <c:axId val="2091276256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2070,7 +2121,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1886785600"/>
+        <c:crossAx val="2091272864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2337,8 +2388,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1885670496"/>
-        <c:axId val="-1885674256"/>
+        <c:axId val="2090115648"/>
+        <c:axId val="2090109168"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2569,8 +2620,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1885680768"/>
-        <c:axId val="-1885678016"/>
+        <c:axId val="2090103120"/>
+        <c:axId val="2090106048"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2592,7 +2643,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="42929C"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2685,11 +2736,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1885670496"/>
-        <c:axId val="-1885674256"/>
+        <c:axId val="2090115648"/>
+        <c:axId val="2090109168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1885680768"/>
+        <c:axId val="2090103120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2732,7 +2783,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885678016"/>
+        <c:crossAx val="2090106048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2740,7 +2791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1885678016"/>
+        <c:axId val="2090106048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2860,12 +2911,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885680768"/>
+        <c:crossAx val="2090103120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1885674256"/>
+        <c:axId val="2090109168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25.0"/>
@@ -2966,12 +3017,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885670496"/>
+        <c:crossAx val="2090115648"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1885670496"/>
+        <c:axId val="2090115648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2980,7 +3031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1885674256"/>
+        <c:crossAx val="2090109168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3226,8 +3277,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1885704400"/>
-        <c:axId val="-1885707520"/>
+        <c:axId val="2090168000"/>
+        <c:axId val="2090164240"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3416,8 +3467,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1886735152"/>
-        <c:axId val="-1886733104"/>
+        <c:axId val="2090157728"/>
+        <c:axId val="2090160480"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3511,11 +3562,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1885704400"/>
-        <c:axId val="-1885707520"/>
+        <c:axId val="2090168000"/>
+        <c:axId val="2090164240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1886735152"/>
+        <c:axId val="2090157728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3558,7 +3609,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1886733104"/>
+        <c:crossAx val="2090160480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3566,7 +3617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1886733104"/>
+        <c:axId val="2090160480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3686,12 +3737,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1886735152"/>
+        <c:crossAx val="2090157728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1885707520"/>
+        <c:axId val="2090164240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30.0"/>
@@ -3793,12 +3844,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885704400"/>
+        <c:crossAx val="2090168000"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1885704400"/>
+        <c:axId val="2090168000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3807,7 +3858,834 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1885707520"/>
+        <c:crossAx val="2090164240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="0"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown Chart For Sprint #5</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task Data'!$A$129</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Completed Tasks</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task Data'!$C$129:$P$129</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2126638016"/>
+        <c:axId val="2126680288"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task Data'!$A$103</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task Data'!$C$126:$P$126</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task Data'!$A$104</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal burndown</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task Data'!$B$127:$O$127</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.42857142857143</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.85714285714286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.28571428571428</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.71428571428571</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.14285714285714</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.57142857142857</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.99999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.42857142857142</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.85714285714285</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.28571428571428</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.714285714285708</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.142857142857137</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.571428571428565</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2054822288"/>
+        <c:axId val="2126765328"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task Data'!$A$128</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Tasks Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="42929C"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task Data'!$C$128:$P$128</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2126638016"/>
+        <c:axId val="2126680288"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2054822288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="&quot;Day&quot;\ \&#10;#0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2126765328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2126765328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Remaining effort</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (hours)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0106619284049409"/>
+              <c:y val="0.363958048275306"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2054822288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2126680288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="30.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Remaining and completed tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.77957124146298"/>
+              <c:y val="0.329852296086731"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2126638016"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="2126638016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2126680288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3972,6 +4850,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5559,6 +6477,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -5650,6 +7084,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>821266</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>148167</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5921,10 +7387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X106"/>
+  <dimension ref="A1:X129"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScale="75" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="T103" sqref="T103"/>
+    <sheetView topLeftCell="A102" zoomScale="75" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="Q136" sqref="Q136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11393,11 +12859,977 @@
         <v>8</v>
       </c>
     </row>
+    <row r="108" spans="1:16" ht="42" x14ac:dyDescent="0.5">
+      <c r="A108" s="122" t="s">
+        <v>111</v>
+      </c>
+      <c r="B108" s="123"/>
+      <c r="C108" s="123"/>
+      <c r="D108" s="123"/>
+      <c r="E108" s="123"/>
+      <c r="F108" s="123"/>
+      <c r="G108" s="123"/>
+      <c r="H108" s="123"/>
+      <c r="I108" s="123"/>
+      <c r="J108" s="123"/>
+      <c r="K108" s="123"/>
+      <c r="L108" s="123"/>
+      <c r="M108" s="123"/>
+      <c r="N108" s="123"/>
+      <c r="O108" s="123"/>
+      <c r="P108" s="124"/>
+    </row>
+    <row r="109" spans="1:16" ht="32" x14ac:dyDescent="0.35">
+      <c r="A109" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="B109" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" s="85" t="s">
+        <v>26</v>
+      </c>
+      <c r="D109" s="86" t="s">
+        <v>27</v>
+      </c>
+      <c r="E109" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="F109" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="G109" s="86" t="s">
+        <v>30</v>
+      </c>
+      <c r="H109" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="I109" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="J109" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="K109" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="L109" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="M109" s="85" t="s">
+        <v>36</v>
+      </c>
+      <c r="N109" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="O109" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="P109" s="86" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A110" s="106" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" s="83"/>
+      <c r="C110" s="75"/>
+      <c r="D110" s="75"/>
+      <c r="E110" s="75"/>
+      <c r="F110" s="75"/>
+      <c r="G110" s="75"/>
+      <c r="H110" s="75"/>
+      <c r="I110" s="75"/>
+      <c r="J110" s="75"/>
+      <c r="K110" s="75"/>
+      <c r="L110" s="75"/>
+      <c r="M110" s="75"/>
+      <c r="N110" s="75"/>
+      <c r="O110" s="75"/>
+      <c r="P110" s="107"/>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A111" s="108" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" s="102">
+        <v>1</v>
+      </c>
+      <c r="C111" s="70">
+        <v>0</v>
+      </c>
+      <c r="D111" s="70">
+        <v>0</v>
+      </c>
+      <c r="E111" s="70">
+        <v>0</v>
+      </c>
+      <c r="F111" s="70">
+        <v>0</v>
+      </c>
+      <c r="G111" s="70">
+        <v>0</v>
+      </c>
+      <c r="H111" s="70">
+        <v>0</v>
+      </c>
+      <c r="I111" s="117">
+        <v>1</v>
+      </c>
+      <c r="J111" s="70">
+        <v>0</v>
+      </c>
+      <c r="K111" s="70">
+        <v>0</v>
+      </c>
+      <c r="L111" s="70">
+        <v>0</v>
+      </c>
+      <c r="M111" s="70">
+        <v>0</v>
+      </c>
+      <c r="N111" s="70">
+        <v>0</v>
+      </c>
+      <c r="O111" s="70">
+        <v>0</v>
+      </c>
+      <c r="P111" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A112" s="108" t="s">
+        <v>114</v>
+      </c>
+      <c r="B112" s="102">
+        <v>1</v>
+      </c>
+      <c r="C112" s="70">
+        <v>0</v>
+      </c>
+      <c r="D112" s="70">
+        <v>0</v>
+      </c>
+      <c r="E112" s="70">
+        <v>0</v>
+      </c>
+      <c r="F112" s="70">
+        <v>0</v>
+      </c>
+      <c r="G112" s="70">
+        <v>0</v>
+      </c>
+      <c r="H112" s="70">
+        <v>0</v>
+      </c>
+      <c r="I112" s="70">
+        <v>0</v>
+      </c>
+      <c r="J112" s="70">
+        <v>0</v>
+      </c>
+      <c r="K112" s="70">
+        <v>0</v>
+      </c>
+      <c r="L112" s="70">
+        <v>0</v>
+      </c>
+      <c r="M112" s="70">
+        <v>0</v>
+      </c>
+      <c r="N112" s="117">
+        <v>1</v>
+      </c>
+      <c r="O112" s="70">
+        <v>0</v>
+      </c>
+      <c r="P112" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A113" s="108" t="s">
+        <v>115</v>
+      </c>
+      <c r="B113" s="102">
+        <v>1</v>
+      </c>
+      <c r="C113" s="70">
+        <v>0</v>
+      </c>
+      <c r="D113" s="70">
+        <v>0</v>
+      </c>
+      <c r="E113" s="70">
+        <v>0</v>
+      </c>
+      <c r="F113" s="70">
+        <v>0</v>
+      </c>
+      <c r="G113" s="70">
+        <v>0</v>
+      </c>
+      <c r="H113" s="70">
+        <v>0</v>
+      </c>
+      <c r="I113" s="70">
+        <v>0</v>
+      </c>
+      <c r="J113" s="70">
+        <v>0</v>
+      </c>
+      <c r="K113" s="70">
+        <v>0</v>
+      </c>
+      <c r="L113" s="70">
+        <v>0</v>
+      </c>
+      <c r="M113" s="70">
+        <v>0</v>
+      </c>
+      <c r="N113" s="117">
+        <v>1</v>
+      </c>
+      <c r="O113" s="70">
+        <v>0</v>
+      </c>
+      <c r="P113" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A114" s="106" t="s">
+        <v>116</v>
+      </c>
+      <c r="B114" s="83"/>
+      <c r="C114" s="75"/>
+      <c r="D114" s="75"/>
+      <c r="E114" s="75"/>
+      <c r="F114" s="75"/>
+      <c r="G114" s="75"/>
+      <c r="H114" s="75"/>
+      <c r="I114" s="75"/>
+      <c r="J114" s="75"/>
+      <c r="K114" s="75"/>
+      <c r="L114" s="75"/>
+      <c r="M114" s="75"/>
+      <c r="N114" s="75"/>
+      <c r="O114" s="75"/>
+      <c r="P114" s="107"/>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A115" s="108" t="s">
+        <v>117</v>
+      </c>
+      <c r="B115" s="102">
+        <v>1</v>
+      </c>
+      <c r="C115" s="70">
+        <v>0</v>
+      </c>
+      <c r="D115" s="70">
+        <v>0</v>
+      </c>
+      <c r="E115" s="70">
+        <v>0</v>
+      </c>
+      <c r="F115" s="70">
+        <v>0</v>
+      </c>
+      <c r="G115" s="70">
+        <v>0</v>
+      </c>
+      <c r="H115" s="70">
+        <v>0</v>
+      </c>
+      <c r="I115" s="117">
+        <v>1</v>
+      </c>
+      <c r="J115" s="70">
+        <v>0</v>
+      </c>
+      <c r="K115" s="70">
+        <v>0</v>
+      </c>
+      <c r="L115" s="70">
+        <v>0</v>
+      </c>
+      <c r="M115" s="70">
+        <v>0</v>
+      </c>
+      <c r="N115" s="70">
+        <v>0</v>
+      </c>
+      <c r="O115" s="70">
+        <v>0</v>
+      </c>
+      <c r="P115" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A116" s="108" t="s">
+        <v>118</v>
+      </c>
+      <c r="B116" s="102">
+        <v>2</v>
+      </c>
+      <c r="C116" s="70">
+        <v>0</v>
+      </c>
+      <c r="D116" s="70">
+        <v>0</v>
+      </c>
+      <c r="E116" s="70">
+        <v>0</v>
+      </c>
+      <c r="F116" s="70">
+        <v>0</v>
+      </c>
+      <c r="G116" s="70">
+        <v>0</v>
+      </c>
+      <c r="H116" s="70">
+        <v>0</v>
+      </c>
+      <c r="I116" s="70">
+        <v>0</v>
+      </c>
+      <c r="J116" s="70">
+        <v>0</v>
+      </c>
+      <c r="K116" s="70">
+        <v>0</v>
+      </c>
+      <c r="L116" s="70">
+        <v>0</v>
+      </c>
+      <c r="M116" s="70">
+        <v>0</v>
+      </c>
+      <c r="N116" s="117">
+        <v>2</v>
+      </c>
+      <c r="O116" s="70">
+        <v>0</v>
+      </c>
+      <c r="P116" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A117" s="108" t="s">
+        <v>119</v>
+      </c>
+      <c r="B117" s="102">
+        <v>1</v>
+      </c>
+      <c r="C117" s="70">
+        <v>0</v>
+      </c>
+      <c r="D117" s="70">
+        <v>0</v>
+      </c>
+      <c r="E117" s="70">
+        <v>0</v>
+      </c>
+      <c r="F117" s="70">
+        <v>0</v>
+      </c>
+      <c r="G117" s="70">
+        <v>0</v>
+      </c>
+      <c r="H117" s="70">
+        <v>0</v>
+      </c>
+      <c r="I117" s="70">
+        <v>0</v>
+      </c>
+      <c r="J117" s="70">
+        <v>0</v>
+      </c>
+      <c r="K117" s="70">
+        <v>0</v>
+      </c>
+      <c r="L117" s="70">
+        <v>0</v>
+      </c>
+      <c r="M117" s="70">
+        <v>0</v>
+      </c>
+      <c r="N117" s="117">
+        <v>1</v>
+      </c>
+      <c r="O117" s="70">
+        <v>0</v>
+      </c>
+      <c r="P117" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A118" s="106" t="s">
+        <v>127</v>
+      </c>
+      <c r="B118" s="83"/>
+      <c r="C118" s="75"/>
+      <c r="D118" s="75"/>
+      <c r="E118" s="75"/>
+      <c r="F118" s="75"/>
+      <c r="G118" s="75"/>
+      <c r="H118" s="75"/>
+      <c r="I118" s="75"/>
+      <c r="J118" s="75"/>
+      <c r="K118" s="75"/>
+      <c r="L118" s="75"/>
+      <c r="M118" s="75"/>
+      <c r="N118" s="75"/>
+      <c r="O118" s="75"/>
+      <c r="P118" s="107"/>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A119" s="108" t="s">
+        <v>120</v>
+      </c>
+      <c r="B119" s="102">
+        <v>1</v>
+      </c>
+      <c r="C119" s="70">
+        <v>0</v>
+      </c>
+      <c r="D119" s="70">
+        <v>0</v>
+      </c>
+      <c r="E119" s="70">
+        <v>0</v>
+      </c>
+      <c r="F119" s="70">
+        <v>0</v>
+      </c>
+      <c r="G119" s="70">
+        <v>0</v>
+      </c>
+      <c r="H119" s="70">
+        <v>0</v>
+      </c>
+      <c r="I119" s="70">
+        <v>0</v>
+      </c>
+      <c r="J119" s="70">
+        <v>0</v>
+      </c>
+      <c r="K119" s="70">
+        <v>0</v>
+      </c>
+      <c r="L119" s="70">
+        <v>0</v>
+      </c>
+      <c r="M119" s="70">
+        <v>0</v>
+      </c>
+      <c r="N119" s="117">
+        <v>1</v>
+      </c>
+      <c r="O119" s="70">
+        <v>0</v>
+      </c>
+      <c r="P119" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A120" s="108" t="s">
+        <v>121</v>
+      </c>
+      <c r="B120" s="102">
+        <v>4</v>
+      </c>
+      <c r="C120" s="70">
+        <v>0</v>
+      </c>
+      <c r="D120" s="70">
+        <v>0</v>
+      </c>
+      <c r="E120" s="70">
+        <v>0</v>
+      </c>
+      <c r="F120" s="70">
+        <v>0</v>
+      </c>
+      <c r="G120" s="70">
+        <v>0</v>
+      </c>
+      <c r="H120" s="70">
+        <v>0</v>
+      </c>
+      <c r="I120" s="70">
+        <v>0</v>
+      </c>
+      <c r="J120" s="70">
+        <v>0</v>
+      </c>
+      <c r="K120" s="70">
+        <v>0</v>
+      </c>
+      <c r="L120" s="70">
+        <v>0</v>
+      </c>
+      <c r="M120" s="70">
+        <v>0</v>
+      </c>
+      <c r="N120" s="117">
+        <v>4</v>
+      </c>
+      <c r="O120" s="70">
+        <v>0</v>
+      </c>
+      <c r="P120" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A121" s="108" t="s">
+        <v>122</v>
+      </c>
+      <c r="B121" s="102">
+        <v>1</v>
+      </c>
+      <c r="C121" s="70">
+        <v>0</v>
+      </c>
+      <c r="D121" s="70">
+        <v>0</v>
+      </c>
+      <c r="E121" s="70">
+        <v>0</v>
+      </c>
+      <c r="F121" s="70">
+        <v>0</v>
+      </c>
+      <c r="G121" s="70">
+        <v>0</v>
+      </c>
+      <c r="H121" s="70">
+        <v>0</v>
+      </c>
+      <c r="I121" s="70">
+        <v>0</v>
+      </c>
+      <c r="J121" s="70">
+        <v>0</v>
+      </c>
+      <c r="K121" s="70">
+        <v>0</v>
+      </c>
+      <c r="L121" s="70">
+        <v>0</v>
+      </c>
+      <c r="M121" s="70">
+        <v>0</v>
+      </c>
+      <c r="N121" s="117">
+        <v>1</v>
+      </c>
+      <c r="O121" s="70">
+        <v>0</v>
+      </c>
+      <c r="P121" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A122" s="106" t="s">
+        <v>123</v>
+      </c>
+      <c r="B122" s="83"/>
+      <c r="C122" s="75"/>
+      <c r="D122" s="75"/>
+      <c r="E122" s="75"/>
+      <c r="F122" s="75"/>
+      <c r="G122" s="75"/>
+      <c r="H122" s="75"/>
+      <c r="I122" s="75"/>
+      <c r="J122" s="75"/>
+      <c r="K122" s="75"/>
+      <c r="L122" s="75"/>
+      <c r="M122" s="75"/>
+      <c r="N122" s="75"/>
+      <c r="O122" s="75"/>
+      <c r="P122" s="107"/>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A123" s="108" t="s">
+        <v>124</v>
+      </c>
+      <c r="B123" s="101">
+        <v>20</v>
+      </c>
+      <c r="C123" s="70">
+        <v>0</v>
+      </c>
+      <c r="D123" s="116">
+        <v>1</v>
+      </c>
+      <c r="E123" s="70">
+        <v>0</v>
+      </c>
+      <c r="F123" s="70">
+        <v>0</v>
+      </c>
+      <c r="G123" s="116">
+        <v>2</v>
+      </c>
+      <c r="H123" s="70">
+        <v>0</v>
+      </c>
+      <c r="I123" s="116">
+        <v>2</v>
+      </c>
+      <c r="J123" s="70">
+        <v>0</v>
+      </c>
+      <c r="K123" s="116">
+        <v>5</v>
+      </c>
+      <c r="L123" s="70">
+        <v>0</v>
+      </c>
+      <c r="M123" s="70">
+        <v>0</v>
+      </c>
+      <c r="N123" s="116">
+        <v>5</v>
+      </c>
+      <c r="O123" s="70">
+        <v>0</v>
+      </c>
+      <c r="P123" s="117">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A124" s="106" t="s">
+        <v>126</v>
+      </c>
+      <c r="B124" s="83"/>
+      <c r="C124" s="75"/>
+      <c r="D124" s="75"/>
+      <c r="E124" s="75"/>
+      <c r="F124" s="75"/>
+      <c r="G124" s="75"/>
+      <c r="H124" s="75"/>
+      <c r="I124" s="75"/>
+      <c r="J124" s="75"/>
+      <c r="K124" s="75"/>
+      <c r="L124" s="75"/>
+      <c r="M124" s="75"/>
+      <c r="N124" s="75"/>
+      <c r="O124" s="75"/>
+      <c r="P124" s="107"/>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A125" s="108" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125" s="101">
+        <v>3</v>
+      </c>
+      <c r="C125" s="70">
+        <v>0</v>
+      </c>
+      <c r="D125" s="116">
+        <v>0.5</v>
+      </c>
+      <c r="E125" s="70">
+        <v>0</v>
+      </c>
+      <c r="F125" s="70">
+        <v>0</v>
+      </c>
+      <c r="G125" s="116">
+        <v>0.5</v>
+      </c>
+      <c r="H125" s="70">
+        <v>0</v>
+      </c>
+      <c r="I125" s="116">
+        <v>0.5</v>
+      </c>
+      <c r="J125" s="70">
+        <v>0</v>
+      </c>
+      <c r="K125" s="116">
+        <v>0.5</v>
+      </c>
+      <c r="L125" s="70">
+        <v>0</v>
+      </c>
+      <c r="M125" s="70">
+        <v>0</v>
+      </c>
+      <c r="N125" s="116">
+        <v>0.5</v>
+      </c>
+      <c r="O125" s="70">
+        <v>0</v>
+      </c>
+      <c r="P125" s="117">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A126" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B126" s="78">
+        <f>SUM(B110:B125)</f>
+        <v>36</v>
+      </c>
+      <c r="C126" s="32">
+        <f>SUM(B126-SUM(C110:C125))</f>
+        <v>36</v>
+      </c>
+      <c r="D126" s="32">
+        <f>SUM(C126-SUM(D110:D125))</f>
+        <v>34.5</v>
+      </c>
+      <c r="E126" s="32">
+        <f>SUM(D126-SUM(E110:E125))</f>
+        <v>34.5</v>
+      </c>
+      <c r="F126" s="32">
+        <f>SUM(E126-SUM(F110:F125))</f>
+        <v>34.5</v>
+      </c>
+      <c r="G126" s="32">
+        <f>SUM(F126-SUM(G110:G125))</f>
+        <v>32</v>
+      </c>
+      <c r="H126" s="32">
+        <f>SUM(G126-SUM(H110:H125))</f>
+        <v>32</v>
+      </c>
+      <c r="I126" s="32">
+        <f>SUM(H126-SUM(I110:I125))</f>
+        <v>27.5</v>
+      </c>
+      <c r="J126" s="32">
+        <f>SUM(I126-SUM(J110:J125))</f>
+        <v>27.5</v>
+      </c>
+      <c r="K126" s="32">
+        <f>SUM(J126-SUM(K110:K125))</f>
+        <v>22</v>
+      </c>
+      <c r="L126" s="32">
+        <f>SUM(K126-SUM(L110:L125))</f>
+        <v>22</v>
+      </c>
+      <c r="M126" s="32">
+        <f>SUM(L126-SUM(M110:M125))</f>
+        <v>22</v>
+      </c>
+      <c r="N126" s="32">
+        <f>SUM(M126-SUM(N110:N125))</f>
+        <v>5.5</v>
+      </c>
+      <c r="O126" s="32">
+        <f>SUM(N126-SUM(O110:O125))</f>
+        <v>5.5</v>
+      </c>
+      <c r="P126" s="32">
+        <f>SUM(O126-SUM(P110:P125))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A127" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B127" s="79">
+        <f>B126</f>
+        <v>36</v>
+      </c>
+      <c r="C127" s="6">
+        <f>B127-$B127/COLUMNS(C109:P109)</f>
+        <v>33.428571428571431</v>
+      </c>
+      <c r="D127" s="6">
+        <f>C127-$B127/COLUMNS(D109:Q109)</f>
+        <v>30.857142857142858</v>
+      </c>
+      <c r="E127" s="6">
+        <f>D127-$B127/COLUMNS(E109:R109)</f>
+        <v>28.285714285714285</v>
+      </c>
+      <c r="F127" s="6">
+        <f>E127-$B127/COLUMNS(F109:S109)</f>
+        <v>25.714285714285712</v>
+      </c>
+      <c r="G127" s="6">
+        <f>F127-$B127/COLUMNS(G109:T109)</f>
+        <v>23.142857142857139</v>
+      </c>
+      <c r="H127" s="6">
+        <f>G127-$B127/COLUMNS(H109:U109)</f>
+        <v>20.571428571428566</v>
+      </c>
+      <c r="I127" s="6">
+        <f>H127-$B127/COLUMNS(I109:V109)</f>
+        <v>17.999999999999993</v>
+      </c>
+      <c r="J127" s="6">
+        <f>I127-$B127/COLUMNS(J109:W109)</f>
+        <v>15.428571428571422</v>
+      </c>
+      <c r="K127" s="6">
+        <f>J127-$B127/COLUMNS(K109:X109)</f>
+        <v>12.857142857142851</v>
+      </c>
+      <c r="L127" s="6">
+        <f>K127-$B127/COLUMNS(L109:Y109)</f>
+        <v>10.285714285714279</v>
+      </c>
+      <c r="M127" s="6">
+        <f>L127-$B127/COLUMNS(M109:Z109)</f>
+        <v>7.7142857142857082</v>
+      </c>
+      <c r="N127" s="6">
+        <f>M127-$B127/COLUMNS(N109:AA109)</f>
+        <v>5.142857142857137</v>
+      </c>
+      <c r="O127" s="6">
+        <f>N127-$B127/COLUMNS(O109:AB109)</f>
+        <v>2.5714285714285654</v>
+      </c>
+      <c r="P127" s="6">
+        <f>O127-$B127/COLUMNS(P109:AC109)</f>
+        <v>-6.2172489379008766E-15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A128" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B128" s="50">
+        <f>COUNTIF(B110:B125, "&gt;0")</f>
+        <v>11</v>
+      </c>
+      <c r="C128" s="50">
+        <f>B128-C129</f>
+        <v>11</v>
+      </c>
+      <c r="D128" s="50">
+        <f>C128-D129</f>
+        <v>11</v>
+      </c>
+      <c r="E128" s="50">
+        <f>D128-E129</f>
+        <v>11</v>
+      </c>
+      <c r="F128" s="50">
+        <f t="shared" ref="F128" si="7">E128-F129</f>
+        <v>11</v>
+      </c>
+      <c r="G128" s="50">
+        <f t="shared" ref="G128" si="8">F128-G129</f>
+        <v>11</v>
+      </c>
+      <c r="H128" s="50">
+        <f t="shared" ref="H128" si="9">G128-H129</f>
+        <v>11</v>
+      </c>
+      <c r="I128" s="50">
+        <f t="shared" ref="I128" si="10">H128-I129</f>
+        <v>9</v>
+      </c>
+      <c r="J128" s="50">
+        <f t="shared" ref="J128" si="11">I128-J129</f>
+        <v>9</v>
+      </c>
+      <c r="K128" s="50">
+        <f t="shared" ref="K128" si="12">J128-K129</f>
+        <v>9</v>
+      </c>
+      <c r="L128" s="50">
+        <f t="shared" ref="L128" si="13">K128-L129</f>
+        <v>9</v>
+      </c>
+      <c r="M128" s="50">
+        <f t="shared" ref="M128" si="14">L128-M129</f>
+        <v>9</v>
+      </c>
+      <c r="N128" s="50">
+        <f t="shared" ref="N128" si="15">M128-N129</f>
+        <v>2</v>
+      </c>
+      <c r="O128" s="50">
+        <f t="shared" ref="O128" si="16">N128-O129</f>
+        <v>2</v>
+      </c>
+      <c r="P128" s="50">
+        <f t="shared" ref="P128" si="17">O128-P129</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A129" s="113" t="s">
+        <v>43</v>
+      </c>
+      <c r="B129" s="114">
+        <v>0</v>
+      </c>
+      <c r="C129" s="114">
+        <v>0</v>
+      </c>
+      <c r="D129" s="114">
+        <v>0</v>
+      </c>
+      <c r="E129" s="114">
+        <v>0</v>
+      </c>
+      <c r="F129" s="114">
+        <v>0</v>
+      </c>
+      <c r="G129" s="114">
+        <v>0</v>
+      </c>
+      <c r="H129" s="114">
+        <v>0</v>
+      </c>
+      <c r="I129" s="114">
+        <v>2</v>
+      </c>
+      <c r="J129" s="114">
+        <v>0</v>
+      </c>
+      <c r="K129" s="114">
+        <v>0</v>
+      </c>
+      <c r="L129" s="114">
+        <v>0</v>
+      </c>
+      <c r="M129" s="114">
+        <v>0</v>
+      </c>
+      <c r="N129" s="114">
+        <v>7</v>
+      </c>
+      <c r="O129" s="114">
+        <v>0</v>
+      </c>
+      <c r="P129" s="115">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A32:W32"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A65:P65"/>
+    <mergeCell ref="A108:P108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11407,8 +13839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="H7" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="P67" sqref="P67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>